<commit_message>
cron added, mat parsing added, and removed json
</commit_message>
<xml_diff>
--- a/mednickdb_pyparse/stagemaps/CAPStudy_stagemap.xlsx
+++ b/mednickdb_pyparse/stagemaps/CAPStudy_stagemap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdyet\UCIGoogleDrive\SleepArchData\StudiesToParse\CAPStudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdyet\GoogleDrive\mednickdb_pyparse\mednickdb_pyparse\stagemaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
added waso, wbso, wase and better stage names
</commit_message>
<xml_diff>
--- a/mednickdb_pyparse/stagemaps/CAPStudy_stagemap.xlsx
+++ b/mednickdb_pyparse/stagemaps/CAPStudy_stagemap.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>mapsfrom</t>
-  </si>
-  <si>
-    <t>meaning</t>
   </si>
   <si>
     <t>mapsto</t>
@@ -39,31 +36,31 @@
     <t>S1</t>
   </si>
   <si>
-    <t>stage 1</t>
-  </si>
-  <si>
     <t>S2</t>
-  </si>
-  <si>
-    <t>stage 2</t>
   </si>
   <si>
     <t>S3</t>
   </si>
   <si>
-    <t>stage 3</t>
-  </si>
-  <si>
     <t>S4</t>
-  </si>
-  <si>
-    <t>stage 4</t>
   </si>
   <si>
     <t>REM</t>
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>stage1</t>
+  </si>
+  <si>
+    <t>stage2</t>
+  </si>
+  <si>
+    <t>sws</t>
+  </si>
+  <si>
+    <t>rem</t>
   </si>
 </sst>
 </file>
@@ -422,113 +419,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.64453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="26" width="7.64453125" customWidth="1"/>
+    <col min="1" max="25" width="7.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1">
-        <v>4</v>
-      </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>